<commit_message>
Refactorred FlightBookingTest and modified data sheet
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData/data.xlsx
+++ b/src/main/resources/TestData/data.xlsx
@@ -3,14 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21029"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A6E2AC6-9B33-4CE6-BA20-C393D7C93834}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{3129E4F6-05BD-46D2-A311-B77A8B7E691F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="4260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Locality</t>
   </si>
@@ -32,6 +33,18 @@
   </si>
   <si>
     <t>1 room, 2 adults</t>
+  </si>
+  <si>
+    <t>From</t>
+  </si>
+  <si>
+    <t>To</t>
+  </si>
+  <si>
+    <t>Bangalore</t>
+  </si>
+  <si>
+    <t>Delhi</t>
   </si>
 </sst>
 </file>
@@ -349,32 +362,45 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.85546875" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>